<commit_message>
to inactivate/activate work node
</commit_message>
<xml_diff>
--- a/i2up/excel/centos1.xlsx
+++ b/i2up/excel/centos1.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CFAAC4-ABD7-6642-8F25-1B489F42046E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FC2137-436F-D946-9223-3C0B071D1AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="500" windowWidth="28140" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="hb_node" sheetId="12" r:id="rId1"/>
-    <sheet name="hb_hb_rule" sheetId="13" r:id="rId2"/>
+    <sheet name="work_node" sheetId="14" r:id="rId1"/>
+    <sheet name="hb_node" sheetId="12" r:id="rId2"/>
+    <sheet name="hb_hb_rule" sheetId="13" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>admin</t>
   </si>
@@ -216,6 +217,45 @@
   </si>
   <si>
     <t>192.168.55.12</t>
+  </si>
+  <si>
+    <t>IP地址</t>
+  </si>
+  <si>
+    <t>192.168.55.11</t>
+  </si>
+  <si>
+    <t>数据端口</t>
+  </si>
+  <si>
+    <t>缓存目录</t>
+  </si>
+  <si>
+    <t>日志目录</t>
+  </si>
+  <si>
+    <t>口令</t>
+  </si>
+  <si>
+    <t>Info@1234</t>
+  </si>
+  <si>
+    <t>节点类型</t>
+  </si>
+  <si>
+    <t>源端节点|备端节点</t>
+  </si>
+  <si>
+    <t>/home/sunxo/i2data/cache/</t>
+  </si>
+  <si>
+    <t>/home/sunxo/i2data/log/</t>
+  </si>
+  <si>
+    <t>名称</t>
+  </si>
+  <si>
+    <t>主机名</t>
   </si>
 </sst>
 </file>
@@ -589,11 +629,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11ABAA26-368D-FC46-AB87-E8C30FC4955B}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="3">
+        <v>26804</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{F258A61E-0518-FB46-B838-432E8795F77A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1505F4D5-7932-7941-8F0B-447A680F701D}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -725,7 +857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEFF414-B0D7-AB46-B6AC-BF59E391BC88}">
   <dimension ref="A1:N3"/>
   <sheetViews>

</xml_diff>

<commit_message>
add mysql to centos1.xlsx
</commit_message>
<xml_diff>
--- a/i2up/excel/centos1.xlsx
+++ b/i2up/excel/centos1.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FC2137-436F-D946-9223-3C0B071D1AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C154B27-D673-D741-B077-F0C6BE6FCC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="500" windowWidth="28140" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="500" windowWidth="28140" windowHeight="15180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work_node" sheetId="14" r:id="rId1"/>
-    <sheet name="hb_node" sheetId="12" r:id="rId2"/>
-    <sheet name="hb_hb_rule" sheetId="13" r:id="rId3"/>
+    <sheet name="msq_node" sheetId="15" r:id="rId2"/>
+    <sheet name="hb_node" sheetId="12" r:id="rId3"/>
+    <sheet name="msq_msq_rule" sheetId="16" r:id="rId4"/>
+    <sheet name="hb_hb_rule" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="68">
   <si>
     <t>admin</t>
   </si>
@@ -256,6 +258,91 @@
   </si>
   <si>
     <t>主机名</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>凭据名称</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>用户名</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>密码</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>默认数据库</t>
+    </r>
+  </si>
+  <si>
+    <t>mysql</t>
+  </si>
+  <si>
+    <t>msq_u</t>
+  </si>
+  <si>
+    <t>msq_c1</t>
+  </si>
+  <si>
+    <t>全量同步</t>
+  </si>
+  <si>
+    <t>全量自定义配置</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>增量同步</t>
+    </r>
+  </si>
+  <si>
+    <t>增量自定义配置</t>
+  </si>
+  <si>
+    <t>fruit</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>msq_u_c1</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -318,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -328,6 +415,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11ABAA26-368D-FC46-AB87-E8C30FC4955B}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -721,11 +809,150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650B1702-B2D0-2940-8DB1-B9F2F3E1CF92}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3306</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3306</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1505F4D5-7932-7941-8F0B-447A680F701D}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -857,11 +1084,135 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661C6D93-948C-C144-87A5-67359A60BCD7}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEFF414-B0D7-AB46-B6AC-BF59E391BC88}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add offline to excel tool
</commit_message>
<xml_diff>
--- a/i2up/excel/centos1.xlsx
+++ b/i2up/excel/centos1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C154B27-D673-D741-B077-F0C6BE6FCC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92E8FFC-2F1A-6D42-8030-342F64D97A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="500" windowWidth="28140" windowHeight="15180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work_node" sheetId="14" r:id="rId1"/>
@@ -18,13 +18,26 @@
     <sheet name="hb_node" sheetId="12" r:id="rId3"/>
     <sheet name="msq_msq_rule" sheetId="16" r:id="rId4"/>
     <sheet name="hb_hb_rule" sheetId="13" r:id="rId5"/>
+    <sheet name="offline_rule" sheetId="17" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
   <si>
     <t>admin</t>
   </si>
@@ -343,6 +356,45 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>msq_u_file_off</t>
+  </si>
+  <si>
+    <t>备端库名</t>
+  </si>
+  <si>
+    <t>源端schema</t>
+  </si>
+  <si>
+    <t>备端schema</t>
+  </si>
+  <si>
+    <t>dump_format_file</t>
+  </si>
+  <si>
+    <t>源端文件目录</t>
+  </si>
+  <si>
+    <t>备端文件目录</t>
+  </si>
+  <si>
+    <t>源端类型</t>
+  </si>
+  <si>
+    <t>备端类型</t>
+  </si>
+  <si>
+    <t>表覆盖策略</t>
+  </si>
+  <si>
+    <t>导出线程数</t>
+  </si>
+  <si>
+    <t>装载线程数</t>
+  </si>
+  <si>
+    <t>truncate</t>
   </si>
 </sst>
 </file>
@@ -1212,7 +1264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEFF414-B0D7-AB46-B6AC-BF59E391BC88}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -1324,4 +1376,142 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8255A9B-D5BA-2743-B59C-2C8292B3483C}">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>